<commit_message>
Adding Main Time Tracking
Adding main time tracking file to Time Tracking Folder
</commit_message>
<xml_diff>
--- a/Time Tracking/CEIS400- WEEK 2 Anaum Syed Time Sheet.xlsx
+++ b/Time Tracking/CEIS400- WEEK 2 Anaum Syed Time Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anaumsyed/Downloads/CEIS400 - GroupC - Week1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d037e0306ecfb5d/Desktop/repos_cloned_here/silver-goggles/Time Tracking/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{2AF6B5BB-0DB3-2245-94FB-599C87562408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10950" yWindow="-14835" windowWidth="16500" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Member One" sheetId="1" r:id="rId1"/>
@@ -1071,22 +1071,22 @@
   </sheetPr>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" customWidth="1"/>
-    <col min="5" max="5" width="47.5" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.44140625" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>10</v>
       </c>
@@ -1095,7 +1095,7 @@
       <c r="D1" s="31"/>
       <c r="E1" s="32"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>18</v>
       </c>
@@ -1104,21 +1104,21 @@
       <c r="D2" s="34"/>
       <c r="E2" s="35"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="33"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="35"/>
     </row>
-    <row r="4" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="29"/>
     </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>19</v>
       </c>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="E5" s="37"/>
     </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="40" t="s">
         <v>21</v>
       </c>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="E6" s="39"/>
     </row>
-    <row r="7" spans="1:5" s="4" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" s="4" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>0</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -1166,7 +1166,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" s="5" customFormat="1" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>45349</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" s="5" customFormat="1" ht="69" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>45350</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" s="5" customFormat="1" ht="69" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>45357</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="E12" s="11"/>
     </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -1252,7 +1252,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -1282,7 +1282,7 @@
       </c>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -1292,7 +1292,7 @@
       </c>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -1304,7 +1304,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="E20" s="19"/>
     </row>
-    <row r="21" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -1324,7 +1324,7 @@
       </c>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -1356,7 +1356,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -1408,7 +1408,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:5" s="5" customFormat="1" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" s="5" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -1428,7 +1428,7 @@
       </c>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="E32" s="11"/>
     </row>
-    <row r="33" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -1448,7 +1448,7 @@
       </c>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -1460,7 +1460,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="E35" s="11"/>
     </row>
-    <row r="36" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="E36" s="11"/>
     </row>
-    <row r="37" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="E37" s="11"/>
     </row>
-    <row r="38" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="E38" s="11"/>
     </row>
-    <row r="39" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="E39" s="19"/>
     </row>
-    <row r="40" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="E40" s="11"/>
     </row>
-    <row r="41" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="E41" s="11"/>
     </row>
-    <row r="42" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="E42" s="11"/>
     </row>
-    <row r="43" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="E43" s="11"/>
     </row>
-    <row r="44" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -1560,7 +1560,7 @@
       </c>
       <c r="E44" s="11"/>
     </row>
-    <row r="45" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -1570,7 +1570,7 @@
       </c>
       <c r="E45" s="11"/>
     </row>
-    <row r="46" spans="1:5" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -1580,7 +1580,7 @@
       </c>
       <c r="E46" s="12"/>
     </row>
-    <row r="47" spans="1:5" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="25" t="s">
         <v>9</v>
       </c>
@@ -1592,7 +1592,7 @@
       </c>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" ht="14" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="48" spans="1:5" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A47:C47"/>
@@ -1623,18 +1623,18 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" customWidth="1"/>
-    <col min="5" max="5" width="47.5" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.44140625" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>10</v>
       </c>
@@ -1643,7 +1643,7 @@
       <c r="D1" s="31"/>
       <c r="E1" s="32"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>6</v>
       </c>
@@ -1652,21 +1652,21 @@
       <c r="D2" s="34"/>
       <c r="E2" s="35"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="33"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="35"/>
     </row>
-    <row r="4" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="29"/>
     </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>7</v>
       </c>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="E5" s="37"/>
     </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="40" t="s">
         <v>8</v>
       </c>
@@ -1688,14 +1688,14 @@
       </c>
       <c r="E6" s="39"/>
     </row>
-    <row r="7" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="42"/>
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
       <c r="D7" s="43"/>
       <c r="E7" s="44"/>
     </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" s="4" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" s="5" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -1724,7 +1724,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -1754,7 +1754,7 @@
       </c>
       <c r="E12" s="11"/>
     </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -1776,7 +1776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -1786,7 +1786,7 @@
       </c>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -1796,7 +1796,7 @@
       </c>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -1828,7 +1828,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -1838,7 +1838,7 @@
       </c>
       <c r="E20" s="19"/>
     </row>
-    <row r="21" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -1848,7 +1848,7 @@
       </c>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -1858,7 +1858,7 @@
       </c>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -1868,7 +1868,7 @@
       </c>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -1880,7 +1880,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -1890,7 +1890,7 @@
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -1900,7 +1900,7 @@
       </c>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -1910,7 +1910,7 @@
       </c>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -1920,7 +1920,7 @@
       </c>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -1932,7 +1932,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -1952,7 +1952,7 @@
       </c>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -1962,7 +1962,7 @@
       </c>
       <c r="E32" s="11"/>
     </row>
-    <row r="33" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -1984,7 +1984,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -1994,7 +1994,7 @@
       </c>
       <c r="E35" s="11"/>
     </row>
-    <row r="36" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="E36" s="11"/>
     </row>
-    <row r="37" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="E37" s="11"/>
     </row>
-    <row r="38" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -2024,7 +2024,7 @@
       </c>
       <c r="E38" s="11"/>
     </row>
-    <row r="39" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -2034,7 +2034,7 @@
       </c>
       <c r="E39" s="19"/>
     </row>
-    <row r="40" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -2044,7 +2044,7 @@
       </c>
       <c r="E40" s="11"/>
     </row>
-    <row r="41" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="E41" s="11"/>
     </row>
-    <row r="42" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -2064,7 +2064,7 @@
       </c>
       <c r="E42" s="11"/>
     </row>
-    <row r="43" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -2074,7 +2074,7 @@
       </c>
       <c r="E43" s="11"/>
     </row>
-    <row r="44" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="E44" s="11"/>
     </row>
-    <row r="45" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="E45" s="11"/>
     </row>
-    <row r="46" spans="1:5" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -2104,7 +2104,7 @@
       </c>
       <c r="E46" s="12"/>
     </row>
-    <row r="47" spans="1:5" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="25" t="s">
         <v>9</v>
       </c>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" ht="14" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="48" spans="1:5" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A47:C47"/>
@@ -2148,18 +2148,18 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" customWidth="1"/>
-    <col min="5" max="5" width="47.5" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.44140625" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>10</v>
       </c>
@@ -2168,7 +2168,7 @@
       <c r="D1" s="31"/>
       <c r="E1" s="32"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>6</v>
       </c>
@@ -2177,21 +2177,21 @@
       <c r="D2" s="34"/>
       <c r="E2" s="35"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="33"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="35"/>
     </row>
-    <row r="4" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="29"/>
     </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>7</v>
       </c>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="E5" s="37"/>
     </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="40" t="s">
         <v>8</v>
       </c>
@@ -2213,14 +2213,14 @@
       </c>
       <c r="E6" s="39"/>
     </row>
-    <row r="7" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="42"/>
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
       <c r="D7" s="43"/>
       <c r="E7" s="44"/>
     </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" s="4" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" s="5" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -2249,7 +2249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -2269,7 +2269,7 @@
       </c>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -2279,7 +2279,7 @@
       </c>
       <c r="E12" s="11"/>
     </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -2301,7 +2301,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -2331,7 +2331,7 @@
       </c>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -2353,7 +2353,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -2363,7 +2363,7 @@
       </c>
       <c r="E20" s="19"/>
     </row>
-    <row r="21" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -2373,7 +2373,7 @@
       </c>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -2383,7 +2383,7 @@
       </c>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -2393,7 +2393,7 @@
       </c>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -2405,7 +2405,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -2425,7 +2425,7 @@
       </c>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -2457,7 +2457,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -2477,7 +2477,7 @@
       </c>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -2487,7 +2487,7 @@
       </c>
       <c r="E32" s="11"/>
     </row>
-    <row r="33" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -2509,7 +2509,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -2519,7 +2519,7 @@
       </c>
       <c r="E35" s="11"/>
     </row>
-    <row r="36" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="E36" s="11"/>
     </row>
-    <row r="37" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -2539,7 +2539,7 @@
       </c>
       <c r="E37" s="11"/>
     </row>
-    <row r="38" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="E38" s="11"/>
     </row>
-    <row r="39" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -2559,7 +2559,7 @@
       </c>
       <c r="E39" s="19"/>
     </row>
-    <row r="40" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="E40" s="11"/>
     </row>
-    <row r="41" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
@@ -2579,7 +2579,7 @@
       </c>
       <c r="E41" s="11"/>
     </row>
-    <row r="42" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="E42" s="11"/>
     </row>
-    <row r="43" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -2599,7 +2599,7 @@
       </c>
       <c r="E43" s="11"/>
     </row>
-    <row r="44" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -2609,7 +2609,7 @@
       </c>
       <c r="E44" s="11"/>
     </row>
-    <row r="45" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="E45" s="11"/>
     </row>
-    <row r="46" spans="1:5" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="E46" s="12"/>
     </row>
-    <row r="47" spans="1:5" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="25" t="s">
         <v>9</v>
       </c>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" ht="14" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="48" spans="1:5" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A47:C47"/>
@@ -2673,18 +2673,18 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" customWidth="1"/>
-    <col min="5" max="5" width="47.5" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.44140625" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>10</v>
       </c>
@@ -2693,7 +2693,7 @@
       <c r="D1" s="31"/>
       <c r="E1" s="32"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>6</v>
       </c>
@@ -2702,21 +2702,21 @@
       <c r="D2" s="34"/>
       <c r="E2" s="35"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="33"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="35"/>
     </row>
-    <row r="4" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="29"/>
     </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>7</v>
       </c>
@@ -2727,7 +2727,7 @@
       </c>
       <c r="E5" s="37"/>
     </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="40" t="s">
         <v>8</v>
       </c>
@@ -2738,14 +2738,14 @@
       </c>
       <c r="E6" s="39"/>
     </row>
-    <row r="7" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="42"/>
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
       <c r="D7" s="43"/>
       <c r="E7" s="44"/>
     </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" s="4" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" s="5" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -2774,7 +2774,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -2794,7 +2794,7 @@
       </c>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -2804,7 +2804,7 @@
       </c>
       <c r="E12" s="11"/>
     </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -2814,7 +2814,7 @@
       </c>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -2826,7 +2826,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -2836,7 +2836,7 @@
       </c>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -2846,7 +2846,7 @@
       </c>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -2866,7 +2866,7 @@
       </c>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -2878,7 +2878,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="E20" s="19"/>
     </row>
-    <row r="21" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -2918,7 +2918,7 @@
       </c>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -2930,7 +2930,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -2950,7 +2950,7 @@
       </c>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -2960,7 +2960,7 @@
       </c>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -2970,7 +2970,7 @@
       </c>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -2982,7 +2982,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -2992,7 +2992,7 @@
       </c>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="E32" s="11"/>
     </row>
-    <row r="33" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -3034,7 +3034,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="E35" s="11"/>
     </row>
-    <row r="36" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -3054,7 +3054,7 @@
       </c>
       <c r="E36" s="11"/>
     </row>
-    <row r="37" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -3064,7 +3064,7 @@
       </c>
       <c r="E37" s="11"/>
     </row>
-    <row r="38" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -3074,7 +3074,7 @@
       </c>
       <c r="E38" s="11"/>
     </row>
-    <row r="39" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -3084,7 +3084,7 @@
       </c>
       <c r="E39" s="19"/>
     </row>
-    <row r="40" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="E40" s="11"/>
     </row>
-    <row r="41" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
@@ -3104,7 +3104,7 @@
       </c>
       <c r="E41" s="11"/>
     </row>
-    <row r="42" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -3114,7 +3114,7 @@
       </c>
       <c r="E42" s="11"/>
     </row>
-    <row r="43" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -3124,7 +3124,7 @@
       </c>
       <c r="E43" s="11"/>
     </row>
-    <row r="44" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -3134,7 +3134,7 @@
       </c>
       <c r="E44" s="11"/>
     </row>
-    <row r="45" spans="1:5" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -3144,7 +3144,7 @@
       </c>
       <c r="E45" s="11"/>
     </row>
-    <row r="46" spans="1:5" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -3154,7 +3154,7 @@
       </c>
       <c r="E46" s="12"/>
     </row>
-    <row r="47" spans="1:5" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="25" t="s">
         <v>9</v>
       </c>
@@ -3166,7 +3166,7 @@
       </c>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" ht="14" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="48" spans="1:5" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A47:C47"/>

</xml_diff>